<commit_message>
Alle Tabellen einheitlich beschriftet zum Einlesen
</commit_message>
<xml_diff>
--- a/Digitale_Woche.xlsx
+++ b/Digitale_Woche.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiman\Documents\Gruppe 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\01_MSc\opencampus_Data Science with R\Gruppenarbeit\Gruppe-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B2B190-6225-48FA-A611-FC4E9839B1E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1AE85-730D-42C4-B323-CDBDA1AE0DFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08F343A9-1196-4254-86E4-B3735B7164A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{08F343A9-1196-4254-86E4-B3735B7164A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Digitale Woche</t>
+    <t>Digitale_Woche</t>
   </si>
 </sst>
 </file>
@@ -392,16 +392,16 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42994</v>
       </c>
@@ -417,7 +417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42995</v>
       </c>
@@ -425,7 +425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42996</v>
       </c>
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42997</v>
       </c>
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42998</v>
       </c>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42999</v>
       </c>
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43000</v>
       </c>
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43001</v>
       </c>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43351</v>
       </c>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43352</v>
       </c>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43353</v>
       </c>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43354</v>
       </c>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43355</v>
       </c>
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43356</v>
       </c>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43357</v>
       </c>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43358</v>
       </c>
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43715</v>
       </c>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43716</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43717</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43718</v>
       </c>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43719</v>
       </c>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43720</v>
       </c>
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43721</v>
       </c>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43722</v>
       </c>

</xml_diff>